<commit_message>
got results tpe search decision tree, lgbm
</commit_message>
<xml_diff>
--- a/results/BaggingClassifier_DecisionTreeClassifier-estimator_df.xlsx
+++ b/results/BaggingClassifier_DecisionTreeClassifier-estimator_df.xlsx
@@ -476,7 +476,309 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Pipeline(steps=[('scaler', MinMaxScaler()),
+          <t>Pipeline(steps=[('scaler',
+                 ColumnTransformer(n_jobs=-1, remainder='passthrough',
+                                   transformers=[('MinMaxScaler',
+                                                  MinMaxScaler(),
+                                                  ['AE_HR', 'AE_V',
+                                                   'AbsOffAxis_HR',
+                                                   'AbsOffAxis_V',
+                                                   'AbsOnAxis_HR',
+                                                   'AbsOnAxis_V', 'BallPath_HR',
+                                                   'BallPath_V', 'CMT_HR',
+                                                   'CMT_V', 'Corrective_HR',
+                                                   'Corrective_V', 'Delta_AE',
+                                                   'Delta_Fullpath', 'Delta_MT',
+                                                   'Delta_OffAxis',
+                                                   'Delta_OnAxis', 'Delta...
+                                                   'MT_V', 'PeakV_HR',
+                                                   'PeakV_V', 'RT_HR', 'RT_V',
+                                                   'TMT_HR', 'TMT_V', 'VE_HR', ...])])),
+                ('selector', RandomUnderSampler(random_state=42)),
+                ('model',
+                 BaggingClassifier(estimator=DecisionTreeClassifier(class_weight='balanced',
+                                                                    criterion='entropy',
+                                                                    max_depth=2,
+                                                                    max_features='sqrt',
+                                                                    min_samples_leaf=4,
+                                                                    min_samples_split=6,
+                                                                    random_state=42),
+                                   n_estimators=5, random_state=42))])</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': ColumnTransformer(n_jobs=-1, remainder='passthrough',
+                  transformers=[('MinMaxScaler', MinMaxScaler(),
+                                 ['AE_HR', 'AE_V', 'AbsOffAxis_HR',
+                                  'AbsOffAxis_V', 'AbsOnAxis_HR', 'AbsOnAxis_V',
+                                  'BallPath_HR', 'BallPath_V', 'CMT_HR',
+                                  'CMT_V', 'Corrective_HR', 'Corrective_V',
+                                  'Delta_AE', 'Delta_Fullpath', 'Delta_MT',
+                                  'Delta_OffAxis', 'Delta_OnAxis', 'Delta_PV',
+                                  'Delta_RT', 'FullPath_HR', 'FullPath_V',
+                                  'MT_HR', 'MT_V', 'PeakV_HR', 'PeakV_V',
+                                  'RT_HR', 'RT_V', 'TMT_HR', 'TMT_V', 'VE_HR', ...])]), 'model__n_estimators': 5, 'model__estimator__min_samples_split': 6, 'model__estimator__min_samples_leaf': 4, 'model__estimator__max_features': 'sqrt', 'model__estimator__max_depth': 2, 'model__estimator__criterion': 'entropy', 'model__estimator__class_weight': 'balanced'}</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>42</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.7435179549604384</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.4037037037037037</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>[1 0 1 0 0 1 1 1 1 1 1 1 1 0 1 0 0 0 1 0 1 1 0 0]</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>[0 1 1 1 1 0 1 0 0 1 1 1 1 1 1 1 1 0 1 0 0 0 1 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Pipeline(steps=[('scaler',
+                 ColumnTransformer(n_jobs=-1, remainder='passthrough',
+                                   transformers=[('MinMaxScaler',
+                                                  MinMaxScaler(),
+                                                  ['AE_HR', 'AE_V',
+                                                   'AbsOffAxis_HR',
+                                                   'AbsOffAxis_V',
+                                                   'AbsOnAxis_HR',
+                                                   'AbsOnAxis_V', 'BallPath_HR',
+                                                   'BallPath_V', 'CMT_HR',
+                                                   'CMT_V', 'Corrective_HR',
+                                                   'Corrective_V', 'Delta_AE',
+                                                   'Delta_Fullpath', 'Delta_MT',
+                                                   'Delta_OffAxis',
+                                                   'Delta_OnAxis', 'Delta...
+                                                   'MT_V', 'PeakV_HR',
+                                                   'PeakV_V', 'RT_HR', 'RT_V',
+                                                   'TMT_HR', 'TMT_V', 'VE_HR', ...])])),
+                ('selector', RandomUnderSampler(random_state=42)),
+                ('model',
+                 BaggingClassifier(estimator=DecisionTreeClassifier(class_weight='balanced',
+                                                                    criterion='entropy',
+                                                                    max_depth=1,
+                                                                    max_features='sqrt',
+                                                                    min_samples_leaf=4,
+                                                                    min_samples_split=6,
+                                                                    random_state=42),
+                                   n_estimators=50, random_state=42))])</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': ColumnTransformer(n_jobs=-1, remainder='passthrough',
+                  transformers=[('MinMaxScaler', MinMaxScaler(),
+                                 ['AE_HR', 'AE_V', 'AbsOffAxis_HR',
+                                  'AbsOffAxis_V', 'AbsOnAxis_HR', 'AbsOnAxis_V',
+                                  'BallPath_HR', 'BallPath_V', 'CMT_HR',
+                                  'CMT_V', 'Corrective_HR', 'Corrective_V',
+                                  'Delta_AE', 'Delta_Fullpath', 'Delta_MT',
+                                  'Delta_OffAxis', 'Delta_OnAxis', 'Delta_PV',
+                                  'Delta_RT', 'FullPath_HR', 'FullPath_V',
+                                  'MT_HR', 'MT_V', 'PeakV_HR', 'PeakV_V',
+                                  'RT_HR', 'RT_V', 'TMT_HR', 'TMT_V', 'VE_HR', ...])]), 'model__n_estimators': 50, 'model__estimator__min_samples_split': 6, 'model__estimator__min_samples_leaf': 4, 'model__estimator__max_features': 'sqrt', 'model__estimator__max_depth': 1, 'model__estimator__criterion': 'entropy', 'model__estimator__class_weight': 'balanced'}</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>69</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.7435179549604384</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.5833333333333334</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>[0 1 1 0 1 0 0 0 1 1 1 0 1 0 1 0 1 0 1 1 0 1 1 1]</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>[1 1 1 0 0 1 0 0 1 0 0 0 1 1 1 0 1 0 1 0 0 0 0 0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Pipeline(steps=[('scaler',
+                 ColumnTransformer(n_jobs=-1, remainder='passthrough',
+                                   transformers=[('MinMaxScaler',
+                                                  MinMaxScaler(),
+                                                  ['AE_HR', 'AE_V',
+                                                   'AbsOffAxis_HR',
+                                                   'AbsOffAxis_V',
+                                                   'AbsOnAxis_HR',
+                                                   'AbsOnAxis_V', 'BallPath_HR',
+                                                   'BallPath_V', 'CMT_HR',
+                                                   'CMT_V', 'Corrective_HR',
+                                                   'Corrective_V', 'Delta_AE',
+                                                   'Delta_Fullpath', 'Delta_MT',
+                                                   'Delta_OffAxis',
+                                                   'Delta_OnAxis', 'Delta...
+                                                   'MT_V', 'PeakV_HR',
+                                                   'PeakV_V', 'RT_HR', 'RT_V',
+                                                   'TMT_HR', 'TMT_V', 'VE_HR', ...])])),
+                ('selector', RandomUnderSampler(random_state=42)),
+                ('model',
+                 BaggingClassifier(estimator=DecisionTreeClassifier(class_weight='balanced',
+                                                                    criterion='entropy',
+                                                                    max_depth=2,
+                                                                    max_features='sqrt',
+                                                                    min_samples_leaf=4,
+                                                                    min_samples_split=6,
+                                                                    random_state=42),
+                                   n_estimators=5, random_state=42))])</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': ColumnTransformer(n_jobs=-1, remainder='passthrough',
+                  transformers=[('MinMaxScaler', MinMaxScaler(),
+                                 ['AE_HR', 'AE_V', 'AbsOffAxis_HR',
+                                  'AbsOffAxis_V', 'AbsOnAxis_HR', 'AbsOnAxis_V',
+                                  'BallPath_HR', 'BallPath_V', 'CMT_HR',
+                                  'CMT_V', 'Corrective_HR', 'Corrective_V',
+                                  'Delta_AE', 'Delta_Fullpath', 'Delta_MT',
+                                  'Delta_OffAxis', 'Delta_OnAxis', 'Delta_PV',
+                                  'Delta_RT', 'FullPath_HR', 'FullPath_V',
+                                  'MT_HR', 'MT_V', 'PeakV_HR', 'PeakV_V',
+                                  'RT_HR', 'RT_V', 'TMT_HR', 'TMT_V', 'VE_HR', ...])]), 'model__n_estimators': 5, 'model__estimator__min_samples_split': 6, 'model__estimator__min_samples_leaf': 4, 'model__estimator__max_features': 'sqrt', 'model__estimator__max_depth': 2, 'model__estimator__criterion': 'entropy', 'model__estimator__class_weight': 'balanced'}</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>23</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.6267148683722655</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.530812324929972</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>[0 0 1 0 0 1 0 1 1 1 1 1 1 1 1 0 0 0 1 0 1 1 1 0]</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>[1 1 1 1 0 1 1 1 1 1 1 0 1 1 1 1 1 1 1 1 1 1 0 0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Pipeline(steps=[('scaler',
+                 ColumnTransformer(n_jobs=-1, remainder='passthrough',
+                                   transformers=[('MinMaxScaler',
+                                                  MinMaxScaler(),
+                                                  ['AE_HR', 'AE_V',
+                                                   'AbsOffAxis_HR',
+                                                   'AbsOffAxis_V',
+                                                   'AbsOnAxis_HR',
+                                                   'AbsOnAxis_V', 'BallPath_HR',
+                                                   'BallPath_V', 'CMT_HR',
+                                                   'CMT_V', 'Corrective_HR',
+                                                   'Corrective_V', 'Delta_AE',
+                                                   'Delta_Fullpath', 'Delta_MT',
+                                                   'Delta_OffAxis',
+                                                   'Delta_OnAxis', 'Delta...
+                                                   'FullPath_V', 'MT_HR',
+                                                   'MT_V', 'PeakV_HR',
+                                                   'PeakV_V', 'RT_HR', 'RT_V',
+                                                   'TMT_HR', 'TMT_V', 'VE_HR', ...])])),
+                ('selector', RandomUnderSampler(random_state=42)),
+                ('model',
+                 BaggingClassifier(estimator=DecisionTreeClassifier(class_weight='balanced',
+                                                                    criterion='entropy',
+                                                                    max_depth=1,
+                                                                    max_features='sqrt',
+                                                                    min_samples_leaf=4,
+                                                                    min_samples_split=6,
+                                                                    random_state=42),
+                                   random_state=42))])</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': ColumnTransformer(n_jobs=-1, remainder='passthrough',
+                  transformers=[('MinMaxScaler', MinMaxScaler(),
+                                 ['AE_HR', 'AE_V', 'AbsOffAxis_HR',
+                                  'AbsOffAxis_V', 'AbsOnAxis_HR', 'AbsOnAxis_V',
+                                  'BallPath_HR', 'BallPath_V', 'CMT_HR',
+                                  'CMT_V', 'Corrective_HR', 'Corrective_V',
+                                  'Delta_AE', 'Delta_Fullpath', 'Delta_MT',
+                                  'Delta_OffAxis', 'Delta_OnAxis', 'Delta_PV',
+                                  'Delta_RT', 'FullPath_HR', 'FullPath_V',
+                                  'MT_HR', 'MT_V', 'PeakV_HR', 'PeakV_V',
+                                  'RT_HR', 'RT_V', 'TMT_HR', 'TMT_V', 'VE_HR', ...])]), 'model__n_estimators': 10, 'model__estimator__min_samples_split': 6, 'model__estimator__min_samples_leaf': 4, 'model__estimator__max_features': 'sqrt', 'model__estimator__max_depth': 1, 'model__estimator__criterion': 'entropy', 'model__estimator__class_weight': 'balanced'}</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>99</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.6597299640777903</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.3693284936479129</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>[0 0 1 1 0 1 1 1 1 0 1 1 0 1 1 0 0 1 0 1 1 0 0 1]</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>[1 0 1 1 1 1 0 1 0 1 0 0 1 0 1 1 1 1 1 0 1 0 1 0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Pipeline(steps=[('scaler',
+                 ColumnTransformer(n_jobs=-1, remainder='passthrough',
+                                   transformers=[('MinMaxScaler',
+                                                  MinMaxScaler(),
+                                                  ['AE_HR', 'AE_V',
+                                                   'AbsOffAxis_HR',
+                                                   'AbsOffAxis_V',
+                                                   'AbsOnAxis_HR',
+                                                   'AbsOnAxis_V', 'BallPath_HR',
+                                                   'BallPath_V', 'CMT_HR',
+                                                   'CMT_V', 'Corrective_HR',
+                                                   'Corrective_V', 'Delta_AE',
+                                                   'Delta_Fullpath', 'Delta_MT',
+                                                   'Delta_OffAxis',
+                                                   'Delta_OnAxis', 'Delta...
+                                                   'MT_V', 'PeakV_HR',
+                                                   'PeakV_V', 'RT_HR', 'RT_V',
+                                                   'TMT_HR', 'TMT_V', 'VE_HR', ...])])),
                 ('selector', RandomUnderSampler(random_state=42)),
                 ('model',
                  BaggingClassifier(estimator=DecisionTreeClassifier(class_weight='balanced',
@@ -489,195 +791,29 @@
                                    n_estimators=200, random_state=42))])</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': MinMaxScaler(), 'model__n_estimators': 200, 'model__estimator__min_samples_split': 6, 'model__estimator__min_samples_leaf': 4, 'model__estimator__max_features': 'sqrt', 'model__estimator__max_depth': 1, 'model__estimator__criterion': 'entropy', 'model__estimator__class_weight': 'balanced'}</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>42</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.6968339307048983</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.4166666666666667</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>[1 0 1 0 0 1 1 1 1 1 1 1 1 0 1 0 0 0 1 0 1 1 0 0]</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>[0 1 1 1 1 0 1 0 0 1 1 1 0 1 1 0 1 0 1 0 0 0 1 1]</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Pipeline(steps=[('scaler', MinMaxScaler()),
-                ('selector', RandomUnderSampler(random_state=42)),
-                ('model',
-                 BaggingClassifier(estimator=DecisionTreeClassifier(class_weight='balanced',
-                                                                    criterion='entropy',
-                                                                    max_depth=1,
-                                                                    max_features='sqrt',
-                                                                    min_samples_leaf=4,
-                                                                    min_samples_split=6,
-                                                                    random_state=42),
-                                   n_estimators=100, random_state=42))])</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': MinMaxScaler(), 'model__n_estimators': 100, 'model__estimator__min_samples_split': 6, 'model__estimator__min_samples_leaf': 4, 'model__estimator__max_features': 'sqrt', 'model__estimator__max_depth': 1, 'model__estimator__criterion': 'entropy', 'model__estimator__class_weight': 'balanced'}</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>69</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.6907872570938308</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.5440917107583775</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>[0 1 1 0 1 0 0 0 1 1 1 0 1 0 1 0 1 0 1 1 0 1 1 1]</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>[1 1 1 0 0 1 0 0 1 0 1 0 1 1 1 0 1 1 1 0 1 0 0 0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Pipeline(steps=[('scaler', MinMaxScaler()),
-                ('selector', RandomUnderSampler(random_state=42)),
-                ('model',
-                 BaggingClassifier(estimator=DecisionTreeClassifier(class_weight='balanced',
-                                                                    criterion='entropy',
-                                                                    max_depth=2,
-                                                                    max_features='sqrt',
-                                                                    min_samples_leaf=4,
-                                                                    min_samples_split=6,
-                                                                    random_state=42),
-                                   random_state=42))])</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': MinMaxScaler(), 'model__n_estimators': 10, 'model__estimator__min_samples_split': 6, 'model__estimator__min_samples_leaf': 4, 'model__estimator__max_features': 'sqrt', 'model__estimator__max_depth': 2, 'model__estimator__criterion': 'entropy', 'model__estimator__class_weight': 'balanced'}</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>23</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.7108993157380253</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.5740740740740741</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>[0 0 1 0 0 1 0 1 1 1 1 1 1 1 1 0 0 0 1 0 1 1 1 0]</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>[0 1 1 0 0 0 1 1 1 1 1 0 1 1 1 1 1 0 1 1 1 0 0 1]</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Pipeline(steps=[('scaler', MinMaxScaler()),
-                ('selector', RandomUnderSampler(random_state=42)),
-                ('model',
-                 BaggingClassifier(estimator=DecisionTreeClassifier(class_weight='balanced',
-                                                                    criterion='entropy',
-                                                                    max_depth=2,
-                                                                    max_features='sqrt',
-                                                                    min_samples_leaf=4,
-                                                                    min_samples_split=6,
-                                                                    random_state=42),
-                                   n_estimators=5, random_state=42))])</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': MinMaxScaler(), 'model__n_estimators': 5, 'model__estimator__min_samples_split': 6, 'model__estimator__min_samples_leaf': 4, 'model__estimator__max_features': 'sqrt', 'model__estimator__max_depth': 2, 'model__estimator__criterion': 'entropy', 'model__estimator__class_weight': 'balanced'}</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>99</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.7273673257023935</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.4534180278281911</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>[0 0 1 1 0 1 1 1 1 0 1 1 0 1 1 0 0 1 0 1 1 0 0 1]</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>[1 0 1 0 0 0 1 1 0 1 0 1 1 1 1 1 1 0 1 1 1 1 0 0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Pipeline(steps=[('scaler', MinMaxScaler()),
-                ('selector', RandomUnderSampler(random_state=42)),
-                ('model',
-                 BaggingClassifier(estimator=DecisionTreeClassifier(class_weight='balanced',
-                                                                    criterion='entropy',
-                                                                    max_depth=4,
-                                                                    max_features='sqrt',
-                                                                    min_samples_leaf=4,
-                                                                    min_samples_split=6,
-                                                                    random_state=42),
-                                   n_estimators=200, random_state=42))])</t>
-        </is>
-      </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': MinMaxScaler(), 'model__n_estimators': 200, 'model__estimator__min_samples_split': 6, 'model__estimator__min_samples_leaf': 4, 'model__estimator__max_features': 'sqrt', 'model__estimator__max_depth': 4, 'model__estimator__criterion': 'entropy', 'model__estimator__class_weight': 'balanced'}</t>
+          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': ColumnTransformer(n_jobs=-1, remainder='passthrough',
+                  transformers=[('MinMaxScaler', MinMaxScaler(),
+                                 ['AE_HR', 'AE_V', 'AbsOffAxis_HR',
+                                  'AbsOffAxis_V', 'AbsOnAxis_HR', 'AbsOnAxis_V',
+                                  'BallPath_HR', 'BallPath_V', 'CMT_HR',
+                                  'CMT_V', 'Corrective_HR', 'Corrective_V',
+                                  'Delta_AE', 'Delta_Fullpath', 'Delta_MT',
+                                  'Delta_OffAxis', 'Delta_OnAxis', 'Delta_PV',
+                                  'Delta_RT', 'FullPath_HR', 'FullPath_V',
+                                  'MT_HR', 'MT_V', 'PeakV_HR', 'PeakV_V',
+                                  'RT_HR', 'RT_V', 'TMT_HR', 'TMT_V', 'VE_HR', ...])]), 'model__n_estimators': 200, 'model__estimator__min_samples_split': 6, 'model__estimator__min_samples_leaf': 4, 'model__estimator__max_features': 'sqrt', 'model__estimator__max_depth': 1, 'model__estimator__criterion': 'entropy', 'model__estimator__class_weight': 'balanced'}</t>
         </is>
       </c>
       <c r="D6" t="n">
         <v>89</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8826889141281694</v>
+        <v>0.7440360090022505</v>
       </c>
       <c r="F6" t="n">
-        <v>0.5</v>
+        <v>0.5440917107583775</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -686,7 +822,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>[0 0 1 1 1 0 0 0 1 0 1 1 1 1 1 1 0 0 1 1 0 1 0 1]</t>
+          <t>[0 0 1 1 1 0 0 0 1 0 1 1 1 1 1 1 0 0 0 1 0 1 0 1]</t>
         </is>
       </c>
     </row>

</xml_diff>